<commit_message>
inetbanking application new version v2 uploaded to github on 9th feb 2019
</commit_message>
<xml_diff>
--- a/src/test/java/com/inetbanking/testData/LoginData.xlsx
+++ b/src/test/java/com/inetbanking/testData/LoginData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -27,28 +27,16 @@
     <t>password</t>
   </si>
   <si>
-    <t>mngr112909</t>
-  </si>
-  <si>
-    <t>tytUreg</t>
-  </si>
-  <si>
-    <t>mngr137319</t>
-  </si>
-  <si>
-    <t>bAdYvyb</t>
-  </si>
-  <si>
-    <t>mngr164225</t>
-  </si>
-  <si>
-    <t>jahetAp</t>
-  </si>
-  <si>
     <t>EnutAje</t>
   </si>
   <si>
     <t>mngr167936</t>
+  </si>
+  <si>
+    <t>mngr177009</t>
+  </si>
+  <si>
+    <t>hubapEv</t>
   </si>
 </sst>
 </file>
@@ -430,7 +418,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -441,7 +429,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -460,18 +448,18 @@
     </row>
     <row r="2" spans="1:2" ht="23.25">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="23.25">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="23.25">
@@ -484,18 +472,18 @@
     </row>
     <row r="5" spans="1:2" ht="23.25">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="23.25">
       <c r="A6" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>